<commit_message>
240722_2 - MC(반출입기, MOMA) Topics, Issue List Update -ing
</commit_message>
<xml_diff>
--- a/박병규/4.IssueList/240722_1_반출입기_MOMA_IssueList_ing.xlsx
+++ b/박병규/4.IssueList/240722_1_반출입기_MOMA_IssueList_ing.xlsx
@@ -140,11 +140,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>데이터의 갱신 신뢰도는 어느정도인지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>갱신주기를 짧게하는 경우 시스템에 미치는 영향</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터의 갱신 주기를 짧게할 수 있는지
+혹은 이벤트 트리거로 변경이 가능한지?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -267,9 +268,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,6 +285,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,38 +841,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.69921875" style="5" customWidth="1"/>
-    <col min="2" max="3" width="8.796875" style="4"/>
-    <col min="4" max="4" width="13.3984375" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20.69921875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="50.69921875" style="4" customWidth="1"/>
-    <col min="8" max="9" width="60.69921875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.796875" style="5"/>
+    <col min="1" max="1" width="3.69921875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="8.796875" style="3"/>
+    <col min="4" max="4" width="13.3984375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="20.69921875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="39.19921875" style="3" customWidth="1"/>
+    <col min="8" max="9" width="60.69921875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1082,11 +1083,11 @@
       <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.4">
@@ -1097,7 +1098,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
@@ -1450,16 +1451,16 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="2:9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>40</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>